<commit_message>
refactor for dense mxts in progress
Former-commit-id: 2ebe87a65f8af01c1ed68cc87de788926ab8e0b4
</commit_message>
<xml_diff>
--- a/examples/study_score_distributions/tal_gata/Effect of different smoothening windows on KS statistic.xlsx
+++ b/examples/study_score_distributions/tal_gata/Effect of different smoothening windows on KS statistic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,11 +525,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2066971096"/>
-        <c:axId val="-2066968008"/>
+        <c:axId val="-2074539256"/>
+        <c:axId val="-2076879160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2066971096"/>
+        <c:axId val="-2074539256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -558,7 +558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066968008"/>
+        <c:crossAx val="-2076879160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -566,7 +566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066968008"/>
+        <c:axId val="-2076879160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -597,7 +597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066971096"/>
+        <c:crossAx val="-2074539256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1008,11 +1008,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2067094424"/>
-        <c:axId val="-2067159992"/>
+        <c:axId val="-2077019608"/>
+        <c:axId val="-2077025208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2067094424"/>
+        <c:axId val="-2077019608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067159992"/>
+        <c:crossAx val="-2077025208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2067159992"/>
+        <c:axId val="-2077025208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -1080,7 +1080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067094424"/>
+        <c:crossAx val="-2077019608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1491,11 +1491,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2061117640"/>
-        <c:axId val="-2061010392"/>
+        <c:axId val="-2077064936"/>
+        <c:axId val="-2077070536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2061117640"/>
+        <c:axId val="-2077064936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1524,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061010392"/>
+        <c:crossAx val="-2077070536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1532,7 +1532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061010392"/>
+        <c:axId val="-2077070536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.3"/>
@@ -1563,7 +1563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061117640"/>
+        <c:crossAx val="-2077064936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2004,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>